<commit_message>
Updates to rating curve and titration curve.
</commit_message>
<xml_diff>
--- a/Outputs/Titration Curve/CO2PPM 07_16.xlsx
+++ b/Outputs/Titration Curve/CO2PPM 07_16.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20346"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20348"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nehemiah\Desktop\Ecuador\Outputs\Titration Curve\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695A0BE9-5E27-462F-915A-7F3EB78ECF22}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{942D77E1-7D2B-4DC0-BCC1-0EA95623FE53}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1811,7 +1811,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11281714785651795"/>
+          <c:y val="0.16708333333333336"/>
+          <c:w val="0.81862729658792655"/>
+          <c:h val="0.62271617089530473"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -21268,8 +21278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="G83" sqref="A1:G111"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -23838,7 +23848,7 @@
   <dimension ref="A1:O111"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>